<commit_message>
Add Compression Sensor to Subsystem Interface
</commit_message>
<xml_diff>
--- a/docs/Subsystem-Interface-Conversions.xlsx
+++ b/docs/Subsystem-Interface-Conversions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>Subsystem</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>Counts per inHg</t>
+  </si>
+  <si>
+    <t>Counts per in</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Compression - Biscuit</t>
   </si>
 </sst>
 </file>
@@ -152,6 +161,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Vacuum</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -324,6 +389,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>inHg</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -386,6 +507,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Counts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -424,6 +601,502 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="410040360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Compression - Biscuit</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$24:$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$24:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$24:$B$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>385</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>461</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>570</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="513178232"/>
+        <c:axId val="513179800"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="513178232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>in</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513179800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="513179800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Counts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="513178232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -512,6 +1185,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1028,20 +1741,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>769620</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1055,6 +2284,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1326,21 +2585,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1372,7 +2631,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9890</v>
+        <v>664</v>
       </c>
       <c r="C2">
         <v>90</v>
@@ -1382,7 +2641,7 @@
       </c>
       <c r="E2">
         <f>(D2-B2)/C2</f>
-        <v>-2.5111111111111111</v>
+        <v>100</v>
       </c>
       <c r="G2">
         <v>-2.5</v>
@@ -1496,7 +2755,7 @@
         <v>12</v>
       </c>
       <c r="B11">
-        <v>700</v>
+        <v>775</v>
       </c>
       <c r="C11">
         <v>35.533000000000001</v>
@@ -1506,7 +2765,7 @@
       </c>
       <c r="E11">
         <f>(B11-D11)/C11</f>
-        <v>18.799988742858751</v>
+        <v>20.910702727042466</v>
       </c>
       <c r="G11">
         <v>0.14099999999999999</v>
@@ -1548,7 +2807,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>800</v>
       </c>
@@ -1556,12 +2815,101 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>900</v>
       </c>
       <c r="C18">
         <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>570</v>
+      </c>
+      <c r="C21">
+        <v>26.561</v>
+      </c>
+      <c r="D21">
+        <v>383.9</v>
+      </c>
+      <c r="E21">
+        <f>(B21-D21)/C21</f>
+        <v>7.006513308986861</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <f>G21*C21+D21</f>
+        <v>383.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>385</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>461</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>518</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>570</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply day unbag changes
</commit_message>
<xml_diff>
--- a/docs/Subsystem-Interface-Conversions.xlsx
+++ b/docs/Subsystem-Interface-Conversions.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marisa_2\Documents\Stryke_Force\FRC\2019-deep-space\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertskalnins/Documents/sf/2019/deepspace/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB75BA-C5C9-ED40-B182-DEAEF0B6E12C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -89,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +155,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -187,7 +194,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -276,7 +282,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -356,6 +361,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DB24-C24F-B3FD-EE1F2307F476}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -415,7 +425,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -533,7 +542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -650,7 +658,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -689,7 +697,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -778,7 +785,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -852,6 +858,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5636-6C4D-83AD-A7FE9F85418A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -911,7 +922,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1029,7 +1039,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2274,7 +2283,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2304,7 +2319,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2584,25 +2605,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +2647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2651,7 +2672,7 @@
         <v>9889</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2676,7 +2697,7 @@
         <v>-15.004000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +2747,7 @@
         <v>31998.400000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -2750,12 +2771,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>775</v>
+        <v>900</v>
       </c>
       <c r="C11">
         <v>35.533000000000001</v>
@@ -2765,7 +2786,7 @@
       </c>
       <c r="E11">
         <f>(B11-D11)/C11</f>
-        <v>20.910702727042466</v>
+        <v>24.428559367348662</v>
       </c>
       <c r="G11">
         <v>0.14099999999999999</v>
@@ -2775,7 +2796,7 @@
         <v>36.990152999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -2783,7 +2804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>500</v>
       </c>
@@ -2791,7 +2812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>600</v>
       </c>
@@ -2799,7 +2820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>700</v>
       </c>
@@ -2807,7 +2828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>800</v>
       </c>
@@ -2815,7 +2836,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>900</v>
       </c>
@@ -2823,7 +2844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2847,7 +2868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2872,7 +2893,7 @@
         <v>383.9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -2880,7 +2901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>385</v>
       </c>
@@ -2888,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>461</v>
       </c>
@@ -2896,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>518</v>
       </c>
@@ -2904,7 +2925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>570</v>
       </c>

</xml_diff>

<commit_message>
Rkalnins/unbag day 2 (#160)
* Add intake, biscuit, elevator checks

* Apply day unbag changes
</commit_message>
<xml_diff>
--- a/docs/Subsystem-Interface-Conversions.xlsx
+++ b/docs/Subsystem-Interface-Conversions.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marisa_2\Documents\Stryke_Force\FRC\2019-deep-space\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertskalnins/Documents/sf/2019/deepspace/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB75BA-C5C9-ED40-B182-DEAEF0B6E12C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -89,7 +96,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +155,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -187,7 +194,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -276,7 +282,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -356,6 +361,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DB24-C24F-B3FD-EE1F2307F476}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -415,7 +425,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -533,7 +542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -650,7 +658,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -689,7 +697,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -778,7 +785,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -852,6 +858,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5636-6C4D-83AD-A7FE9F85418A}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -911,7 +922,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1029,7 +1039,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2274,7 +2283,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2304,7 +2319,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2584,25 +2605,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2626,7 +2647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2651,7 +2672,7 @@
         <v>9889</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -2676,7 +2697,7 @@
         <v>-15.004000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +2721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2726,7 +2747,7 @@
         <v>31998.400000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -2750,12 +2771,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>775</v>
+        <v>900</v>
       </c>
       <c r="C11">
         <v>35.533000000000001</v>
@@ -2765,7 +2786,7 @@
       </c>
       <c r="E11">
         <f>(B11-D11)/C11</f>
-        <v>20.910702727042466</v>
+        <v>24.428559367348662</v>
       </c>
       <c r="G11">
         <v>0.14099999999999999</v>
@@ -2775,7 +2796,7 @@
         <v>36.990152999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>13</v>
       </c>
@@ -2783,7 +2804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>500</v>
       </c>
@@ -2791,7 +2812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>600</v>
       </c>
@@ -2799,7 +2820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16">
         <v>700</v>
       </c>
@@ -2807,7 +2828,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>800</v>
       </c>
@@ -2815,7 +2836,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>900</v>
       </c>
@@ -2823,7 +2844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2847,7 +2868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2872,7 +2893,7 @@
         <v>383.9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -2880,7 +2901,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24">
         <v>385</v>
       </c>
@@ -2888,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B25">
         <v>461</v>
       </c>
@@ -2896,7 +2917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B26">
         <v>518</v>
       </c>
@@ -2904,7 +2925,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27">
         <v>570</v>
       </c>

</xml_diff>

<commit_message>
Optimize ball ground and coconut pickup
</commit_message>
<xml_diff>
--- a/docs/Subsystem-Interface-Conversions.xlsx
+++ b/docs/Subsystem-Interface-Conversions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertskalnins/Documents/sf/2019/deepspace/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAB75BA-C5C9-ED40-B182-DEAEF0B6E12C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BF0C61-395C-D740-8DAF-E4B431B41426}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2609,7 +2609,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2726,7 +2726,7 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>4900</v>
+        <v>17415</v>
       </c>
       <c r="C7">
         <v>1120</v>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="E7">
         <f>(B7+D7)/C7</f>
-        <v>8.375</v>
+        <v>19.549107142857142</v>
       </c>
       <c r="G7">
         <v>32.57</v>

</xml_diff>

<commit_message>
Begin tuning pickup and place
</commit_message>
<xml_diff>
--- a/docs/Subsystem-Interface-Conversions.xlsx
+++ b/docs/Subsystem-Interface-Conversions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertskalnins/Documents/sf/2019/deepspace/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD48C5A2-D699-6943-90B2-9078749270BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{273574F6-A572-CE47-8B2E-B91C7A8D094A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2609,7 +2609,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2789,11 +2789,11 @@
         <v>24.428559367348662</v>
       </c>
       <c r="G11">
-        <v>21.6</v>
+        <v>2.5</v>
       </c>
       <c r="H11">
         <f>G11*C11+D11</f>
-        <v>799.4928000000001</v>
+        <v>120.81250000000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add pre elims changes
</commit_message>
<xml_diff>
--- a/docs/Subsystem-Interface-Conversions.xlsx
+++ b/docs/Subsystem-Interface-Conversions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertskalnins/Documents/sf/2019/deepspace/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8C1747-443B-4943-B48C-24E8466C11B2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA980A4-1087-EA4E-A4C2-5AFE2CFF9099}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="33600" windowHeight="18220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2609,7 +2610,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2665,11 +2666,11 @@
         <v>112.65555555555555</v>
       </c>
       <c r="G2">
-        <v>115.6</v>
+        <v>115.85</v>
       </c>
       <c r="H2">
         <f>-G2*C2+D2</f>
-        <v>-740</v>
+        <v>-762.5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>